<commit_message>
Ajeitando a Matriz de Adjacencias
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -248,10 +249,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -271,6 +272,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -279,59 +287,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,6 +308,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -362,9 +325,31 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,7 +370,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,13 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,8 +399,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,7 +431,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,31 +503,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,37 +533,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,13 +551,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,7 +569,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,61 +605,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,39 +622,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -697,6 +665,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -721,151 +713,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1748,7 +1749,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -7688,7 +7689,7 @@
       <c r="A63" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -7696,10 +7697,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7724,9 +7725,10 @@
     <col min="20" max="20" width="16" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
     <col min="22" max="22" width="12.4285714285714" customWidth="1"/>
+    <col min="23" max="23" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" spans="2:22">
+    <row r="1" ht="12.75" customHeight="1" spans="2:23">
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
@@ -7790,8 +7792,11 @@
       <c r="V1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1" spans="1:22">
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -7858,8 +7863,11 @@
       <c r="V2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7926,8 +7934,11 @@
       <c r="V3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" spans="1:22">
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -7994,8 +8005,11 @@
       <c r="V4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -8062,8 +8076,11 @@
       <c r="V5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -8130,8 +8147,11 @@
       <c r="V6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -8198,8 +8218,11 @@
       <c r="V7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -8266,8 +8289,11 @@
       <c r="V8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1" spans="1:22">
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="16.5" customHeight="1" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -8334,8 +8360,11 @@
       <c r="V9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" ht="19.5" customHeight="1" spans="1:22">
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="19.5" customHeight="1" spans="1:23">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -8402,8 +8431,11 @@
       <c r="V10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:22">
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -8470,8 +8502,11 @@
       <c r="V11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -8538,8 +8573,11 @@
       <c r="V12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -8606,8 +8644,11 @@
       <c r="V13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -8674,8 +8715,11 @@
       <c r="V14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -8742,8 +8786,11 @@
       <c r="V15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -8810,8 +8857,11 @@
       <c r="V16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -8878,8 +8928,11 @@
       <c r="V17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -8946,8 +8999,11 @@
       <c r="V18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -9014,8 +9070,11 @@
       <c r="V19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -9082,8 +9141,11 @@
       <c r="V20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
@@ -9150,8 +9212,11 @@
       <c r="V21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -9218,6 +9283,80 @@
       <c r="V22">
         <v>0</v>
       </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1"/>
@@ -9262,7 +9401,23 @@
       <c r="A55" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações para exibição de caminho
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -248,10 +248,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -271,7 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,46 +285,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,6 +322,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -361,10 +346,32 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,17 +392,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -407,15 +406,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,13 +430,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,19 +448,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,103 +538,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,25 +562,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,18 +641,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,159 +706,166 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1748,7 +1748,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -7688,7 +7688,7 @@
       <c r="A63" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -7699,7 +7699,7 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9219,6 +9219,74 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+    </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1"/>
     </row>
@@ -9262,7 +9330,7 @@
       <c r="A55" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>